<commit_message>
28.05.18 today last sales Update
</commit_message>
<xml_diff>
--- a/May/Daily Sales Info/All Details/28.05.19/DSR Wise Sales Report.xlsx
+++ b/May/Daily Sales Info/All Details/28.05.19/DSR Wise Sales Report.xlsx
@@ -52,7 +52,7 @@
     <t>-------------------------------------------------------</t>
   </si>
   <si>
-    <t>Date:27.05.19</t>
+    <t>Date:28.05.19</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -557,13 +557,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>87425</v>
+        <v>121160</v>
       </c>
       <c r="C6" s="2">
-        <v>81</v>
+        <v>44</v>
       </c>
       <c r="D6" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -571,13 +571,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>61300</v>
+        <v>72980</v>
       </c>
       <c r="C7" s="2">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D7" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -585,10 +585,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>31205</v>
+        <v>39345</v>
       </c>
       <c r="C8" s="2">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2">
         <v>8</v>
@@ -608,15 +608,15 @@
       </c>
       <c r="B10" s="4">
         <f>SUM(B6:B8)</f>
-        <v>179930</v>
+        <v>233485</v>
       </c>
       <c r="C10" s="4">
         <f>SUM(C6:C8)</f>
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="D10" s="4">
         <f>SUM(D6:D8)</f>
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>